<commit_message>
Updated and moved workflows from GetTransactionData to Process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\Calculate Client Security Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3117AEC-740F-4692-A63E-ACB6A6D2E61E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F352284-131F-4FF6-86D7-31F04DE1DE98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>